<commit_message>
constrain and conflict check
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -1,30 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="5808" windowWidth="16212" xWindow="480" yWindow="108"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,16 +60,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -342,208 +378,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E7" activeCellId="0" pane="topLeft" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="2" width="8.529999999999999"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Course</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Prof</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Slots</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="2" s="3">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>IC210</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Ramesh</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Ramesh</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Slot A</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="3" s="3">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>IC211</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Suresh</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Slot B</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>IC245</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Suresh</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>No Slots</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="4" s="3">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>IC212</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Himesh</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Himesh</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Slot C</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="5" s="3">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>IC213</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Mahesh</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Mahesh</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Slot D</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="6" s="3">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>IC214</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Rajesh</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Rajesh</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>No Slots</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>IC345</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Mahesh</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="7" s="3">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>IC215</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Ganesh</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Ganesh</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>No Slots</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>IC546</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Rajesh</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="8" s="3">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>IC216</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Mangesh</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Mangesh</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>No Slots</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>IC456</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Ganesh</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>No Slots</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>IC908</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Mangesh</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>No Slots</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>IC377</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="9" s="3">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>IC217</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Naresh</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Naresh</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>Slot H</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="2" width="8.529999999999999"/>
+  </cols>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="2" width="8.529999999999999"/>
+  </cols>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed names and initiated Main Interface
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>

</xml_diff>